<commit_message>
I think final commit :)
</commit_message>
<xml_diff>
--- a/SystemData.xlsx
+++ b/SystemData.xlsx
@@ -13,7 +13,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4354" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="19">
+  <si>
+    <t>COMPANIES</t>
+  </si>
+  <si>
+    <t>Total Assets</t>
+  </si>
+  <si>
+    <t>Current Assets</t>
+  </si>
+  <si>
+    <t>Net Income</t>
+  </si>
+  <si>
+    <t>Net Sales</t>
+  </si>
+  <si>
+    <t>Net Credit Sales</t>
+  </si>
+  <si>
+    <t>Average Total Assets</t>
+  </si>
+  <si>
+    <t>Gross profit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Total liabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Liabilities
+</t>
+  </si>
+  <si>
+    <t>Cost of Goods sold</t>
+  </si>
+  <si>
+    <t>Owners equity</t>
+  </si>
+  <si>
+    <t>Average shareholder’s equity</t>
+  </si>
+  <si>
+    <t>Market Price per share</t>
+  </si>
+  <si>
+    <t>Earnings per share</t>
+  </si>
+  <si>
+    <t>Cash dividends</t>
+  </si>
   <si>
     <t/>
   </si>
@@ -29,12 +78,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -51,9 +109,15 @@
   <cellStyleXfs count="1">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -266,1910 +330,1915 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:AF21"/>
+  <dimension ref="A1:AF21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U2" t="s">
-        <v>0</v>
-      </c>
-      <c r="V2" t="s">
-        <v>0</v>
-      </c>
-      <c r="W2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="B2" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>623.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>213.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>2100.0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>8443.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE6" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE7" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE10" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE11" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE15" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE16" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE17" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE18" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="W21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="X21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Z21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AC21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AE21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FINAL COMMIT(DONT COMMIT AGAIN)
</commit_message>
<xml_diff>
--- a/SystemData.xlsx
+++ b/SystemData.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3123" uniqueCount="19">
   <si>
     <t>COMPANIES</t>
   </si>
@@ -388,52 +388,97 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>30000.0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>20000.0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>623.0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>213.0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>2100.0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>8443.0</v>
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">

</xml_diff>